<commit_message>
Fikset kommunesammenslåing slik at final_data_24 forhåpentligvis er feilfri
</commit_message>
<xml_diff>
--- a/Data/Vinmonopolet/Kommuneendringer_24.xlsx
+++ b/Data/Vinmonopolet/Kommuneendringer_24.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9884e02f7050b840/Skrivebord/Spring_2025/Ban440/Eksamen/BAN440-Term-Paper/BAN440-Term-Paper/Data/Vinmonopolet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhhit-my.sharepoint.com/personal/sander_eriksen_student_nhh_no/Documents/NHH/8. semester/BAN440/Term paper/BAN440---Term-Paper/Data/Vinmonopolet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F24E2DBA-60B4-4231-A777-F0DA407D987C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{F24E2DBA-60B4-4231-A777-F0DA407D987C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99D035DD-4389-416C-9321-0A7101BCFFDE}"/>
   <bookViews>
-    <workbookView xWindow="8970" yWindow="1815" windowWidth="38700" windowHeight="15345" xr2:uid="{047F2BAD-5723-468F-ACC8-F63F1B1D3250}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{047F2BAD-5723-468F-ACC8-F63F1B1D3250}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1116,16 +1116,16 @@
   <dimension ref="A1:B119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B119"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>45292</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>44927</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1253,7 +1253,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>41</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>81</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>83</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>89</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>93</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>95</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>97</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>99</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>101</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>103</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>105</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>107</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>109</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>111</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>113</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>115</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>117</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>119</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>121</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>123</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>125</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>127</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>129</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>131</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>133</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>135</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>137</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>139</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>141</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>143</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>145</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>147</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>149</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>151</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>153</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>155</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>157</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>159</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>161</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>163</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>165</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>167</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>169</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>171</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>173</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>175</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>177</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>179</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>181</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>183</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>185</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>187</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>189</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>191</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>193</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>195</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>197</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>199</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>201</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>203</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>205</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>207</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>209</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>211</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>213</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>215</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>217</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>219</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>221</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>223</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>225</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>227</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>229</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>231</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>233</v>
       </c>

</xml_diff>